<commit_message>
fixed tracking, locked APR
</commit_message>
<xml_diff>
--- a/144F20/Topic 3/QR_2-3_Tech_Template.xlsx
+++ b/144F20/Topic 3/QR_2-3_Tech_Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\richard.ketchersid\OneDrive - GCU Employees\Course Materials\git\Teaching\144F20\Topic 3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="10_ncr:80_{D05394CE-6BE2-4CBA-9938-D304B64A0FF6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{55582A18-81D4-4991-A1C1-18449555D399}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:80_{369E1462-62EC-41B4-8C82-D8F0964F6AE1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="732" yWindow="732" windowWidth="20796" windowHeight="11424" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="696" yWindow="1332" windowWidth="22344" windowHeight="11628" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Interest" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
   </sheets>
   <calcPr calcId="191029" concurrentCalc="0"/>
   <customWorkbookViews>
-    <customWorkbookView name="Richard Ketchersid - Personal View" guid="{155D4935-5B0D-4D9B-9526-5391F2A5AE7E}" mergeInterval="0" personalView="1" xWindow="110" yWindow="26" windowWidth="1862" windowHeight="969" tabRatio="500" activeSheetId="1" showComments="commIndAndComment"/>
+    <customWorkbookView name="Richard Ketchersid - Personal View" guid="{155D4935-5B0D-4D9B-9526-5391F2A5AE7E}" mergeInterval="0" personalView="1" xWindow="58" yWindow="111" windowWidth="1862" windowHeight="969" tabRatio="500" activeSheetId="1"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -874,10 +874,6 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="10" fontId="0" fillId="5" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="5" borderId="31" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
@@ -986,6 +982,10 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="5" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2117,6 +2117,27 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{B7639928-BEDD-4808-AE9F-8753A44600E6}">
+  <header guid="{B7639928-BEDD-4808-AE9F-8753A44600E6}" dateTime="2020-11-19T14:00:18" maxSheetId="3" userName="Richard Ketchersid" r:id="rId1">
+    <sheetIdMap count="2">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+    </sheetIdMap>
+  </header>
+</headers>
+</file>
+
+<file path=xl/revisions/revisionLog1.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac"/>
+</file>
+
+<file path=xl/revisions/userNames.xml><?xml version="1.0" encoding="utf-8"?>
+<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="1">
+  <userInfo guid="{B7639928-BEDD-4808-AE9F-8753A44600E6}" name="Richard Ketchersid" id="-1739526094" dateTime="2020-11-19T14:00:18"/>
+</users>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -2382,8 +2403,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="184" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14:D14"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="184" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18:D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
@@ -2401,34 +2422,34 @@
   <sheetData>
     <row r="1" spans="1:10" ht="16.2" thickBot="1"/>
     <row r="2" spans="1:10" ht="33" customHeight="1" thickBot="1">
-      <c r="B2" s="56" t="s">
+      <c r="B2" s="55" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="57"/>
-      <c r="D2" s="57"/>
-      <c r="E2" s="57"/>
-      <c r="F2" s="57"/>
-      <c r="G2" s="58"/>
+      <c r="C2" s="56"/>
+      <c r="D2" s="56"/>
+      <c r="E2" s="56"/>
+      <c r="F2" s="56"/>
+      <c r="G2" s="57"/>
     </row>
     <row r="3" spans="1:10" ht="16.2" thickTop="1">
-      <c r="B3" s="59"/>
-      <c r="C3" s="60"/>
-      <c r="D3" s="60"/>
-      <c r="E3" s="60"/>
-      <c r="F3" s="60"/>
-      <c r="G3" s="61"/>
-      <c r="I3" s="54" t="s">
+      <c r="B3" s="58"/>
+      <c r="C3" s="59"/>
+      <c r="D3" s="59"/>
+      <c r="E3" s="59"/>
+      <c r="F3" s="59"/>
+      <c r="G3" s="60"/>
+      <c r="I3" s="53" t="s">
         <v>7</v>
       </c>
-      <c r="J3" s="55"/>
+      <c r="J3" s="54"/>
     </row>
     <row r="4" spans="1:10">
-      <c r="B4" s="59"/>
-      <c r="C4" s="60"/>
-      <c r="D4" s="60"/>
-      <c r="E4" s="60"/>
-      <c r="F4" s="60"/>
-      <c r="G4" s="61"/>
+      <c r="B4" s="58"/>
+      <c r="C4" s="59"/>
+      <c r="D4" s="59"/>
+      <c r="E4" s="59"/>
+      <c r="F4" s="59"/>
+      <c r="G4" s="60"/>
       <c r="I4" s="5" t="s">
         <v>8</v>
       </c>
@@ -2437,12 +2458,12 @@
       </c>
     </row>
     <row r="5" spans="1:10">
-      <c r="B5" s="59"/>
-      <c r="C5" s="60"/>
-      <c r="D5" s="60"/>
-      <c r="E5" s="60"/>
-      <c r="F5" s="60"/>
-      <c r="G5" s="61"/>
+      <c r="B5" s="58"/>
+      <c r="C5" s="59"/>
+      <c r="D5" s="59"/>
+      <c r="E5" s="59"/>
+      <c r="F5" s="59"/>
+      <c r="G5" s="60"/>
       <c r="I5" s="7" t="s">
         <v>10</v>
       </c>
@@ -2451,12 +2472,12 @@
       </c>
     </row>
     <row r="6" spans="1:10" ht="16.2" thickBot="1">
-      <c r="B6" s="62"/>
-      <c r="C6" s="63"/>
-      <c r="D6" s="63"/>
-      <c r="E6" s="63"/>
-      <c r="F6" s="63"/>
-      <c r="G6" s="64"/>
+      <c r="B6" s="61"/>
+      <c r="C6" s="62"/>
+      <c r="D6" s="62"/>
+      <c r="E6" s="62"/>
+      <c r="F6" s="62"/>
+      <c r="G6" s="63"/>
       <c r="I6" s="9" t="s">
         <v>12</v>
       </c>
@@ -2465,14 +2486,14 @@
       </c>
     </row>
     <row r="7" spans="1:10" ht="16.2" thickBot="1">
-      <c r="B7" s="74" t="s">
+      <c r="B7" s="73" t="s">
         <v>30</v>
       </c>
-      <c r="C7" s="75"/>
-      <c r="D7" s="75"/>
-      <c r="E7" s="75"/>
-      <c r="F7" s="75"/>
-      <c r="G7" s="76"/>
+      <c r="C7" s="74"/>
+      <c r="D7" s="74"/>
+      <c r="E7" s="74"/>
+      <c r="F7" s="74"/>
+      <c r="G7" s="75"/>
       <c r="I7" s="10" t="s">
         <v>14</v>
       </c>
@@ -2481,14 +2502,14 @@
       </c>
     </row>
     <row r="8" spans="1:10" ht="16.2" customHeight="1" thickBot="1">
-      <c r="B8" s="65" t="s">
+      <c r="B8" s="64" t="s">
         <v>31</v>
       </c>
-      <c r="C8" s="66"/>
-      <c r="D8" s="66"/>
-      <c r="E8" s="66"/>
-      <c r="F8" s="66"/>
-      <c r="G8" s="67"/>
+      <c r="C8" s="65"/>
+      <c r="D8" s="65"/>
+      <c r="E8" s="65"/>
+      <c r="F8" s="65"/>
+      <c r="G8" s="66"/>
       <c r="I8" s="11" t="s">
         <v>16</v>
       </c>
@@ -2497,20 +2518,20 @@
       </c>
     </row>
     <row r="9" spans="1:10" ht="16.2" thickTop="1">
-      <c r="B9" s="68"/>
-      <c r="C9" s="69"/>
-      <c r="D9" s="69"/>
-      <c r="E9" s="69"/>
-      <c r="F9" s="69"/>
-      <c r="G9" s="70"/>
+      <c r="B9" s="67"/>
+      <c r="C9" s="68"/>
+      <c r="D9" s="68"/>
+      <c r="E9" s="68"/>
+      <c r="F9" s="68"/>
+      <c r="G9" s="69"/>
     </row>
     <row r="10" spans="1:10" ht="15.6" customHeight="1" thickBot="1">
-      <c r="B10" s="71"/>
-      <c r="C10" s="72"/>
-      <c r="D10" s="72"/>
-      <c r="E10" s="72"/>
-      <c r="F10" s="72"/>
-      <c r="G10" s="73"/>
+      <c r="B10" s="70"/>
+      <c r="C10" s="71"/>
+      <c r="D10" s="71"/>
+      <c r="E10" s="71"/>
+      <c r="F10" s="71"/>
+      <c r="G10" s="72"/>
     </row>
     <row r="11" spans="1:10" ht="16.2" thickBot="1">
       <c r="B11" s="20"/>
@@ -2529,42 +2550,42 @@
         <v>26</v>
       </c>
       <c r="E12" s="48"/>
-      <c r="F12" s="50"/>
-      <c r="G12" s="77" t="s">
+      <c r="F12" s="49"/>
+      <c r="G12" s="76" t="s">
         <v>32</v>
       </c>
-      <c r="H12" s="78"/>
+      <c r="H12" s="77"/>
     </row>
     <row r="13" spans="1:10" ht="16.2" thickBot="1">
       <c r="D13" s="3" t="s">
         <v>27</v>
       </c>
       <c r="E13" s="48"/>
-      <c r="F13" s="50"/>
-      <c r="G13" s="79"/>
-      <c r="H13" s="80"/>
+      <c r="F13" s="49"/>
+      <c r="G13" s="78"/>
+      <c r="H13" s="79"/>
     </row>
     <row r="14" spans="1:10" ht="16.2" thickBot="1">
-      <c r="A14" s="81" t="s">
+      <c r="A14" s="80" t="s">
         <v>56</v>
       </c>
-      <c r="B14" s="82"/>
-      <c r="C14" s="83" t="s">
+      <c r="B14" s="81"/>
+      <c r="C14" s="82" t="s">
         <v>57</v>
       </c>
-      <c r="D14" s="84"/>
+      <c r="D14" s="83"/>
       <c r="E14" s="41"/>
       <c r="F14" s="42"/>
     </row>
     <row r="15" spans="1:10" ht="16.2" thickBot="1">
-      <c r="D15" s="52" t="s">
+      <c r="D15" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="E15" s="52"/>
-      <c r="F15" s="53" t="s">
+      <c r="E15" s="51"/>
+      <c r="F15" s="52" t="s">
         <v>6</v>
       </c>
-      <c r="G15" s="53"/>
+      <c r="G15" s="52"/>
     </row>
     <row r="16" spans="1:10" s="15" customFormat="1" ht="31.2">
       <c r="A16" s="13" t="s">
@@ -2616,7 +2637,7 @@
       <c r="A18" s="48">
         <v>600</v>
       </c>
-      <c r="B18" s="49" t="str">
+      <c r="B18" s="84" t="str">
         <f>IF(C14="Full Name (5 letters)", "Fill C14",5%+SIGN(0.5-Sheet1!C15)*(1%+Sheet1!D20/100))</f>
         <v>Fill C14</v>
       </c>
@@ -2876,10 +2897,10 @@
       <c r="F44"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="QoS5bMTgt1giztW+3cm/4Evo8F2eUYfvsIr/XXSJm8TJCN+RwEWPmX3d5RUqhevnMKg1FU3aSQA26tvMdJlx5Q==" saltValue="psu2jzljY5jsulJF4hlQWQ==" spinCount="100000" sheet="1" formatCells="0"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="2A/rww8Nqv4fK2TlQVl65mtizyEtTrhoBgoSzfI0L61rev8ObAQvBrmKe9v54Be415tIbuhAPt3rUgjGXM0kEQ==" saltValue="5kSmu5Ey9AYQWjMTHx1V6A==" spinCount="100000" sheet="1" formatCells="0"/>
   <customSheetViews>
-    <customSheetView guid="{155D4935-5B0D-4D9B-9526-5391F2A5AE7E}" scale="130" topLeftCell="A13">
-      <selection activeCell="G12" sqref="G12:H13"/>
+    <customSheetView guid="{155D4935-5B0D-4D9B-9526-5391F2A5AE7E}" scale="130" topLeftCell="A16">
+      <selection activeCell="D18" sqref="D18:D24"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
     </customSheetView>
@@ -3678,7 +3699,7 @@
       <c r="A13" t="s">
         <v>35</v>
       </c>
-      <c r="B13" s="51">
+      <c r="B13" s="50">
         <f t="shared" ref="B13:B33" ca="1" si="3">MOD(B12*F$11+F$12,F$13)</f>
         <v>22800</v>
       </c>
@@ -3753,7 +3774,7 @@
       <c r="A14" t="s">
         <v>36</v>
       </c>
-      <c r="B14" s="51">
+      <c r="B14" s="50">
         <f t="shared" ca="1" si="3"/>
         <v>31753</v>
       </c>
@@ -3825,7 +3846,7 @@
       <c r="A15" t="s">
         <v>37</v>
       </c>
-      <c r="B15" s="51">
+      <c r="B15" s="50">
         <f t="shared" ca="1" si="3"/>
         <v>15886</v>
       </c>
@@ -3897,7 +3918,7 @@
       <c r="A16" t="s">
         <v>38</v>
       </c>
-      <c r="B16" s="51">
+      <c r="B16" s="50">
         <f t="shared" ca="1" si="3"/>
         <v>24623</v>
       </c>
@@ -3969,7 +3990,7 @@
       <c r="A17" t="s">
         <v>39</v>
       </c>
-      <c r="B17" s="51">
+      <c r="B17" s="50">
         <f t="shared" ca="1" si="3"/>
         <v>30268</v>
       </c>
@@ -4041,7 +4062,7 @@
       <c r="A18" t="s">
         <v>40</v>
       </c>
-      <c r="B18" s="51">
+      <c r="B18" s="50">
         <f t="shared" ca="1" si="3"/>
         <v>20421</v>
       </c>
@@ -4062,7 +4083,7 @@
       <c r="A19" t="s">
         <v>41</v>
       </c>
-      <c r="B19" s="51">
+      <c r="B19" s="50">
         <f t="shared" ca="1" si="3"/>
         <v>11546</v>
       </c>
@@ -4083,7 +4104,7 @@
       <c r="A20" t="s">
         <v>42</v>
       </c>
-      <c r="B20" s="51">
+      <c r="B20" s="50">
         <f t="shared" ca="1" si="3"/>
         <v>20555</v>
       </c>
@@ -4104,7 +4125,7 @@
       <c r="A21" t="s">
         <v>43</v>
       </c>
-      <c r="B21" s="51">
+      <c r="B21" s="50">
         <f t="shared" ca="1" si="3"/>
         <v>14888</v>
       </c>
@@ -4125,7 +4146,7 @@
       <c r="A22" t="s">
         <v>44</v>
       </c>
-      <c r="B22" s="51">
+      <c r="B22" s="50">
         <f t="shared" ca="1" si="3"/>
         <v>9025</v>
       </c>
@@ -4141,13 +4162,13 @@
         <f t="shared" ca="1" si="6"/>
         <v>1</v>
       </c>
-      <c r="M22" s="51"/>
+      <c r="M22" s="50"/>
     </row>
     <row r="23" spans="1:23">
       <c r="A23" t="s">
         <v>45</v>
       </c>
-      <c r="B23" s="51">
+      <c r="B23" s="50">
         <f t="shared" ca="1" si="3"/>
         <v>230</v>
       </c>
@@ -4163,13 +4184,13 @@
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
-      <c r="M23" s="51"/>
+      <c r="M23" s="50"/>
     </row>
     <row r="24" spans="1:23">
       <c r="A24" t="s">
         <v>46</v>
       </c>
-      <c r="B24" s="51">
+      <c r="B24" s="50">
         <f t="shared" ca="1" si="3"/>
         <v>9767</v>
       </c>
@@ -4185,13 +4206,13 @@
         <f t="shared" ca="1" si="6"/>
         <v>1</v>
       </c>
-      <c r="M24" s="51"/>
+      <c r="M24" s="50"/>
     </row>
     <row r="25" spans="1:23">
       <c r="A25" t="s">
         <v>47</v>
       </c>
-      <c r="B25" s="51">
+      <c r="B25" s="50">
         <f t="shared" ca="1" si="3"/>
         <v>20692</v>
       </c>
@@ -4207,13 +4228,13 @@
         <f t="shared" ca="1" si="6"/>
         <v>3</v>
       </c>
-      <c r="M25" s="51"/>
+      <c r="M25" s="50"/>
     </row>
     <row r="26" spans="1:23">
       <c r="A26" t="s">
         <v>48</v>
       </c>
-      <c r="B26" s="51">
+      <c r="B26" s="50">
         <f t="shared" ca="1" si="3"/>
         <v>12925</v>
       </c>
@@ -4229,13 +4250,13 @@
         <f t="shared" ca="1" si="6"/>
         <v>1</v>
       </c>
-      <c r="M26" s="51"/>
+      <c r="M26" s="50"/>
     </row>
     <row r="27" spans="1:23">
       <c r="A27" t="s">
         <v>49</v>
       </c>
-      <c r="B27" s="51">
+      <c r="B27" s="50">
         <f t="shared" ca="1" si="3"/>
         <v>17778</v>
       </c>
@@ -4251,13 +4272,13 @@
         <f t="shared" ca="1" si="6"/>
         <v>3</v>
       </c>
-      <c r="M27" s="51"/>
+      <c r="M27" s="50"/>
     </row>
     <row r="28" spans="1:23">
       <c r="A28" t="s">
         <v>50</v>
       </c>
-      <c r="B28" s="51">
+      <c r="B28" s="50">
         <f t="shared" ca="1" si="3"/>
         <v>32195</v>
       </c>
@@ -4273,13 +4294,13 @@
         <f t="shared" ca="1" si="6"/>
         <v>4</v>
       </c>
-      <c r="M28" s="51"/>
+      <c r="M28" s="50"/>
     </row>
     <row r="29" spans="1:23">
       <c r="A29" t="s">
         <v>51</v>
       </c>
-      <c r="B29" s="51">
+      <c r="B29" s="50">
         <f t="shared" ca="1" si="3"/>
         <v>9792</v>
       </c>
@@ -4295,13 +4316,13 @@
         <f t="shared" ca="1" si="6"/>
         <v>1</v>
       </c>
-      <c r="M29" s="51"/>
+      <c r="M29" s="50"/>
     </row>
     <row r="30" spans="1:23">
       <c r="A30" t="s">
         <v>52</v>
       </c>
-      <c r="B30" s="51">
+      <c r="B30" s="50">
         <f t="shared" ca="1" si="3"/>
         <v>31097</v>
       </c>
@@ -4317,13 +4338,13 @@
         <f t="shared" ca="1" si="6"/>
         <v>4</v>
       </c>
-      <c r="M30" s="51"/>
+      <c r="M30" s="50"/>
     </row>
     <row r="31" spans="1:23">
       <c r="A31" t="s">
         <v>53</v>
       </c>
-      <c r="B31" s="51">
+      <c r="B31" s="50">
         <f t="shared" ca="1" si="3"/>
         <v>18110</v>
       </c>
@@ -4339,13 +4360,13 @@
         <f t="shared" ca="1" si="6"/>
         <v>3</v>
       </c>
-      <c r="M31" s="51"/>
+      <c r="M31" s="50"/>
     </row>
     <row r="32" spans="1:23">
       <c r="A32" t="s">
         <v>54</v>
       </c>
-      <c r="B32" s="51">
+      <c r="B32" s="50">
         <f t="shared" ca="1" si="3"/>
         <v>13087</v>
       </c>
@@ -4361,13 +4382,13 @@
         <f t="shared" ca="1" si="6"/>
         <v>1</v>
       </c>
-      <c r="M32" s="51"/>
+      <c r="M32" s="50"/>
     </row>
     <row r="33" spans="1:13">
       <c r="A33" t="s">
         <v>55</v>
       </c>
-      <c r="B33" s="51">
+      <c r="B33" s="50">
         <f t="shared" ca="1" si="3"/>
         <v>26220</v>
       </c>
@@ -4383,48 +4404,48 @@
         <f t="shared" ca="1" si="6"/>
         <v>4</v>
       </c>
-      <c r="M33" s="51"/>
+      <c r="M33" s="50"/>
     </row>
     <row r="34" spans="1:13">
-      <c r="M34" s="51"/>
+      <c r="M34" s="50"/>
     </row>
     <row r="35" spans="1:13">
-      <c r="M35" s="51"/>
+      <c r="M35" s="50"/>
     </row>
     <row r="36" spans="1:13">
-      <c r="M36" s="51"/>
+      <c r="M36" s="50"/>
     </row>
     <row r="37" spans="1:13">
-      <c r="M37" s="51"/>
+      <c r="M37" s="50"/>
     </row>
     <row r="38" spans="1:13">
-      <c r="M38" s="51"/>
+      <c r="M38" s="50"/>
     </row>
     <row r="39" spans="1:13">
-      <c r="M39" s="51"/>
+      <c r="M39" s="50"/>
     </row>
     <row r="40" spans="1:13">
-      <c r="M40" s="51"/>
+      <c r="M40" s="50"/>
     </row>
     <row r="41" spans="1:13">
-      <c r="M41" s="51"/>
+      <c r="M41" s="50"/>
     </row>
     <row r="42" spans="1:13">
-      <c r="M42" s="51"/>
+      <c r="M42" s="50"/>
     </row>
     <row r="43" spans="1:13">
-      <c r="M43" s="51"/>
+      <c r="M43" s="50"/>
     </row>
     <row r="44" spans="1:13">
-      <c r="M44" s="51"/>
+      <c r="M44" s="50"/>
     </row>
     <row r="45" spans="1:13">
-      <c r="M45" s="51"/>
+      <c r="M45" s="50"/>
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{155D4935-5B0D-4D9B-9526-5391F2A5AE7E}">
-      <selection activeCell="B6" sqref="B6"/>
+    <customSheetView guid="{155D4935-5B0D-4D9B-9526-5391F2A5AE7E}" state="hidden">
+      <selection activeCell="D12" sqref="D12"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
   </customSheetViews>

</xml_diff>